<commit_message>
add updateToDb func to updateExcel func, add a plugin to filter signed jars
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5643" uniqueCount="38">
   <si>
     <t>Boxes/Checks</t>
   </si>
@@ -136,6 +136,16 @@
   </si>
   <si>
     <t>No Critical Alarms</t>
+  </si>
+  <si>
+    <t>P4:INC000005135152: Wrong schedule on 'True Crime' (154)[Last Update: Raised a new GN case : 01575811 to address title mismatch.]</t>
+  </si>
+  <si>
+    <t>P4: INC000005135676: 01573557|[IE]DTV|14:00|Poster Missing in On Demand | Prime Boxset | Kids+Movies [Last Update: VNOC seeking for an update from GN for the remaining posters to be published]</t>
+  </si>
+  <si>
+    <t>P4:INC000005135152: Wrong schedule on 'True Crime' (154)[Last Update: Raised a new GN case : 01575811 to address title mismatch.]
+P2:kjsdbk</t>
   </si>
 </sst>
 </file>
@@ -554,13 +564,13 @@
         <v>13</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>13</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>13</v>
@@ -586,31 +596,31 @@
         <v>16</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>17</v>
@@ -621,7 +631,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>13</v>
@@ -648,7 +658,7 @@
         <v>13</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -656,7 +666,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>13</v>
@@ -691,22 +701,22 @@
         <v>20</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>13</v>
@@ -726,22 +736,22 @@
         <v>21</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>13</v>
@@ -761,22 +771,22 @@
         <v>22</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>13</v>
@@ -796,7 +806,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>13</v>
@@ -831,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>13</v>
@@ -866,10 +876,10 @@
         <v>25</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>13</v>
@@ -890,10 +900,10 @@
         <v>13</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -901,7 +911,7 @@
         <v>26</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>13</v>
@@ -936,7 +946,7 @@
         <v>27</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>13</v>
@@ -971,7 +981,7 @@
         <v>28</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>13</v>
@@ -1006,22 +1016,22 @@
         <v>29</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s" s="0">
         <v>13</v>
@@ -1041,22 +1051,22 @@
         <v>30</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s" s="0">
         <v>13</v>
@@ -1076,22 +1086,22 @@
         <v>31</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>13</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s" s="0">
         <v>13</v>
@@ -1111,7 +1121,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>13</v>
@@ -1146,16 +1156,16 @@
         <v>33</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s" s="0">
         <v>13</v>
@@ -1164,10 +1174,10 @@
         <v>13</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>13</v>

</xml_diff>